<commit_message>
Update lecture to use '複合参照' terminology
Replaced all instances of '混合参照' with '複合参照' in the lecture materials to standardize terminology. Updated related explanations and examples in the markdown, Excel, and PDF files.
</commit_message>
<xml_diff>
--- a/MCfCL-05-Lecture/05_Ref.xlsx
+++ b/MCfCL-05-Lecture/05_Ref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tetsu\github\2025-SIT-MCfCL\MCfCL-05-Lecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tetsu/GitHub/shimizu-sit/2025-SIT-MCfCL/MCfCL-05-Lecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB05C0BD-9D7D-42FA-B5A4-0843FAE23C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49B6F80-E907-514B-A1F0-A7FC49547046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15945" yWindow="11670" windowWidth="21390" windowHeight="13920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15940" yWindow="11680" windowWidth="21400" windowHeight="13920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="税込" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>日付</t>
   </si>
@@ -64,15 +64,22 @@
   <si>
     <t>割引率</t>
   </si>
+  <si>
+    <t>割引後金額</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">ワリビキゴ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">キンガク </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,7 +177,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -184,7 +191,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -494,7 +501,7 @@
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -505,7 +512,7 @@
     <col min="8" max="8" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,7 +536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
@@ -541,7 +548,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -551,7 +558,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
@@ -561,7 +568,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -571,7 +578,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
@@ -581,7 +588,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -591,7 +598,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
@@ -601,7 +608,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
@@ -611,7 +618,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
@@ -621,7 +628,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
@@ -644,12 +651,12 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -660,7 +667,7 @@
     <col min="8" max="8" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -677,14 +684,14 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
@@ -696,7 +703,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -706,7 +713,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
@@ -716,7 +723,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -726,7 +733,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
@@ -736,7 +743,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -746,7 +753,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
@@ -756,7 +763,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
@@ -766,7 +773,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
@@ -776,7 +783,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
@@ -796,16 +803,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="10" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="22" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -835,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="22" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -850,7 +857,7 @@
       <c r="J2" s="8"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="22" customHeight="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -864,7 +871,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="22" customHeight="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -878,7 +885,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="22" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -892,7 +899,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="22" customHeight="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -906,7 +913,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="22" customHeight="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -920,7 +927,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="22" customHeight="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -934,7 +941,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="22" customHeight="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -948,7 +955,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="22" customHeight="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>

</xml_diff>